<commit_message>
My Class Work done on 11 th July (Tuesday)
</commit_message>
<xml_diff>
--- a/Business Intelligence  Fundamentals (Dhaval Sir)/Dhaval Sir (Class Practice).xlsx
+++ b/Business Intelligence  Fundamentals (Dhaval Sir)/Dhaval Sir (Class Practice).xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achyut Sharma\Documents\Business Intelligence  Fundamentals (Dhaval Sir)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achyut Sharma\Documents\Data Sem 5\Business Intelligence  Fundamentals (Dhaval Sir)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC5BFC7-D78A-46AB-AD98-7D7ABCE517B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5984D54D-7F69-46F2-8D47-0F681E8C6E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise 1(27 June 23)" sheetId="1" r:id="rId1"/>
     <sheet name="Exercise 2 (4 July 23)" sheetId="2" r:id="rId2"/>
-    <sheet name="Exercise 3 Q.1(4 July 23)" sheetId="3" r:id="rId3"/>
-    <sheet name="Exercise 3 Q.2(4 July 23)" sheetId="4" r:id="rId4"/>
+    <sheet name="Exercise 3 Q.1(6 July 23 Thur)" sheetId="3" r:id="rId3"/>
+    <sheet name="Exercise 3 Q.2(6 July 23Thur)" sheetId="4" r:id="rId4"/>
     <sheet name="Exercise 3 Q.3(4 July 23)" sheetId="5" r:id="rId5"/>
     <sheet name="Exercise 3 Q.4(4 July 23)" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="314">
   <si>
     <t>Roll No.</t>
   </si>
@@ -954,6 +954,33 @@
   </si>
   <si>
     <t>No.Of Mondays = COUNTIF (Day_Name ,"Monday")</t>
+  </si>
+  <si>
+    <t>LOOKUP Function And Index Match</t>
+  </si>
+  <si>
+    <t>(Horizontal Lookup)</t>
+  </si>
+  <si>
+    <t>HLOOKUP is used when attributes in column.</t>
+  </si>
+  <si>
+    <t>VLOOKUP is used when attributes are in rows.</t>
+  </si>
+  <si>
+    <t>Use here VLOOKUP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for drag drop lock </t>
+  </si>
+  <si>
+    <t>table array</t>
+  </si>
+  <si>
+    <t>using f4</t>
+  </si>
+  <si>
+    <t>then drag drop</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1089,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1126,11 +1153,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1176,6 +1242,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1983,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8860A8-A8BD-4701-89FC-D0883AD75BB0}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -2652,18 +2725,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A468B79F-181A-4FE7-BD7B-354CCF492C7F}">
-  <dimension ref="C2:J98"/>
+  <dimension ref="C1:J98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView topLeftCell="C84" workbookViewId="0">
+      <selection activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>305</v>
+      </c>
+    </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>80</v>
@@ -5193,20 +5272,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3417819-BE25-444A-8B3F-BDDB719BE575}">
-  <dimension ref="E4:O24"/>
+  <dimension ref="A2:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="6:21" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F4" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F6" s="9" t="s">
         <v>80</v>
       </c>
@@ -5220,100 +5307,216 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F7" s="6">
         <v>3</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="6" t="str">
+        <f>VLOOKUP(F7,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,4,FALSE)</f>
+        <v>Laura</v>
+      </c>
+      <c r="H7" s="6" t="str">
+        <f>VLOOKUP(F7,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,3,FALSE)</f>
+        <v>Canada</v>
+      </c>
+      <c r="I7" s="7">
+        <f>VLOOKUP(F7,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,7,)</f>
+        <v>34459</v>
+      </c>
+    </row>
+    <row r="8" spans="6:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F8" s="6">
         <v>25</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="6" t="str">
+        <f>VLOOKUP(F8,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,4,)</f>
+        <v>Wojtek</v>
+      </c>
+      <c r="H8" s="6" t="str">
+        <f>VLOOKUP(F8,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,3,)</f>
+        <v>Canada</v>
+      </c>
+      <c r="I8" s="7">
+        <f>VLOOKUP(F8,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,7,)</f>
+        <v>31467</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="T8" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="U8" s="15"/>
+    </row>
+    <row r="9" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F9" s="6">
         <v>34</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="6" t="str">
+        <f>VLOOKUP(F9,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,4,)</f>
+        <v>Eric</v>
+      </c>
+      <c r="H9" s="6" t="str">
+        <f>VLOOKUP(F9,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,3,)</f>
+        <v>Canada</v>
+      </c>
+      <c r="I9" s="7">
+        <f>VLOOKUP(F9,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,7,)</f>
+        <v>33045</v>
+      </c>
+    </row>
+    <row r="10" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F10" s="6">
         <v>45</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="6" t="str">
+        <f>VLOOKUP(F10,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,4,)</f>
+        <v>Maxim</v>
+      </c>
+      <c r="H10" s="6" t="str">
+        <f>VLOOKUP(F10,'Exercise 3 Q.1(6 July 23 Thur)'!$C2:$J98,3,)</f>
+        <v>Canada</v>
+      </c>
+      <c r="I10" s="7">
+        <f>VLOOKUP(F10,'Exercise 3 Q.1(6 July 23 Thur)'!$C2:$J98,7,)</f>
+        <v>31921</v>
+      </c>
+    </row>
+    <row r="11" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F11" s="6">
         <v>57</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="6" t="str">
+        <f>VLOOKUP(F11,'Exercise 3 Q.1(6 July 23 Thur)'!$C2:J$98,4,)</f>
+        <v>Nicole</v>
+      </c>
+      <c r="H11" s="6" t="str">
+        <f>VLOOKUP(F11,'Exercise 3 Q.1(6 July 23 Thur)'!$C3:$J99,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I11" s="7">
+        <f>VLOOKUP(F11,'Exercise 3 Q.1(6 July 23 Thur)'!$C3:$J99,7,)</f>
+        <v>34508</v>
+      </c>
+    </row>
+    <row r="12" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F12" s="6">
         <v>65</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G12" s="6" t="str">
+        <f>VLOOKUP(F12,'Exercise 3 Q.1(6 July 23 Thur)'!$C3:J$98,4,)</f>
+        <v>Kelly</v>
+      </c>
+      <c r="H12" s="6" t="str">
+        <f>VLOOKUP(F12,'Exercise 3 Q.1(6 July 23 Thur)'!$C4:$J100,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I12" s="7">
+        <f>VLOOKUP(F12,'Exercise 3 Q.1(6 July 23 Thur)'!$C4:$J100,7,)</f>
+        <v>35062</v>
+      </c>
+    </row>
+    <row r="13" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F13" s="6">
         <v>71</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="6" t="str">
+        <f>VLOOKUP(F13,'Exercise 3 Q.1(6 July 23 Thur)'!$C4:J$98,4,)</f>
+        <v>Lee</v>
+      </c>
+      <c r="H13" s="6" t="str">
+        <f>VLOOKUP(F13,'Exercise 3 Q.1(6 July 23 Thur)'!$C5:$J101,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I13" s="7">
+        <f>VLOOKUP(F13,'Exercise 3 Q.1(6 July 23 Thur)'!$C5:$J101,7,)</f>
+        <v>34447</v>
+      </c>
+    </row>
+    <row r="14" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F14" s="6">
         <v>79</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="6" t="str">
+        <f>VLOOKUP(F14,'Exercise 3 Q.1(6 July 23 Thur)'!$C5:J$98,4,)</f>
+        <v>Matt</v>
+      </c>
+      <c r="H14" s="6" t="str">
+        <f>VLOOKUP(F14,'Exercise 3 Q.1(6 July 23 Thur)'!$C6:$J102,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I14" s="7">
+        <f>VLOOKUP(F14,'Exercise 3 Q.1(6 July 23 Thur)'!$C6:$J102,7,)</f>
+        <v>30883</v>
+      </c>
+    </row>
+    <row r="15" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F15" s="6">
         <v>82</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G15" s="6" t="str">
+        <f>VLOOKUP(F15,'Exercise 3 Q.1(6 July 23 Thur)'!$C6:J$98,4,)</f>
+        <v>Ryan</v>
+      </c>
+      <c r="H15" s="6" t="str">
+        <f>VLOOKUP(F15,'Exercise 3 Q.1(6 July 23 Thur)'!$C7:$J103,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I15" s="7">
+        <f>VLOOKUP(F15,'Exercise 3 Q.1(6 July 23 Thur)'!$C7:$J103,7,)</f>
+        <v>31275</v>
+      </c>
+    </row>
+    <row r="16" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F16" s="6">
         <v>86</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="G16" s="6" t="str">
+        <f>VLOOKUP(F16,'Exercise 3 Q.1(6 July 23 Thur)'!$C7:J$98,4,)</f>
+        <v>Brandon</v>
+      </c>
+      <c r="H16" s="6" t="str">
+        <f>VLOOKUP(F16,'Exercise 3 Q.1(6 July 23 Thur)'!$C8:$J104,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I16" s="7">
+        <f>VLOOKUP(F16,'Exercise 3 Q.1(6 July 23 Thur)'!$C$8:$J$104,7,)</f>
+        <v>33319</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F17" s="6">
         <v>90</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="20" spans="5:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="G17" s="6" t="str">
+        <f>VLOOKUP(F17,'Exercise 3 Q.1(6 July 23 Thur)'!$C8:J$98,4,)</f>
+        <v>Bobby</v>
+      </c>
+      <c r="H17" s="6" t="str">
+        <f>VLOOKUP(F17,'Exercise 3 Q.1(6 July 23 Thur)'!$C9:$J105,3,)</f>
+        <v>USA</v>
+      </c>
+      <c r="I17" s="7">
+        <f>VLOOKUP(F17,'Exercise 3 Q.1(6 July 23 Thur)'!$C$8:$J$104,7,)</f>
+        <v>32202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="E20" s="12" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E21" s="11" t="s">
         <v>275</v>
       </c>
@@ -5345,7 +5548,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E22" s="11" t="s">
         <v>278</v>
       </c>
@@ -5367,8 +5570,20 @@
       <c r="L22" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <f>HLOOKUP(H21,E21:J24,4,)</f>
+        <v>90</v>
+      </c>
+      <c r="N22">
+        <f>HLOOKUP(L22,$E$21:$J$24,3,)</f>
+        <v>50</v>
+      </c>
+      <c r="O22" t="str">
+        <f>HLOOKUP(L22,$E$21:$J$24,2,)</f>
+        <v>c</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E23" s="11" t="s">
         <v>277</v>
       </c>
@@ -5390,8 +5605,20 @@
       <c r="L23" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <f>HLOOKUP(F21,E21:J24,4,)</f>
+        <v>56</v>
+      </c>
+      <c r="N23">
+        <f>HLOOKUP(L23,$E$21:$J$24,3,)</f>
+        <v>45</v>
+      </c>
+      <c r="O23" t="str">
+        <f>HLOOKUP(L23,$E$21:$J$24,2,)</f>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E24" s="11" t="s">
         <v>276</v>
       </c>
@@ -5409,6 +5636,16 @@
       </c>
       <c r="J24" s="11">
         <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -5418,13 +5655,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5922DC4-94E9-454B-BBB5-FED1D6ACACBB}">
-  <dimension ref="H3:U12"/>
+  <dimension ref="H3:U18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="8:21" x14ac:dyDescent="0.3">
       <c r="H3" s="8" t="s">
@@ -5449,10 +5689,10 @@
       </c>
     </row>
     <row r="6" spans="8:21" x14ac:dyDescent="0.3">
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -5594,6 +5834,9 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mysql 13-14 July Notes
</commit_message>
<xml_diff>
--- a/Business Intelligence  Fundamentals (Dhaval Sir)/Dhaval Sir (Class Practice).xlsx
+++ b/Business Intelligence  Fundamentals (Dhaval Sir)/Dhaval Sir (Class Practice).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achyut Sharma\Documents\Data Sem 5\Business Intelligence  Fundamentals (Dhaval Sir)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5984D54D-7F69-46F2-8D47-0F681E8C6E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E309E1-6DA4-45C3-9301-6A78E1126F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise 1(27 June 23)" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="315">
   <si>
     <t>Roll No.</t>
   </si>
@@ -981,6 +981,9 @@
   </si>
   <si>
     <t>then drag drop</t>
+  </si>
+  <si>
+    <t>Index match</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1225,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1231,6 +1233,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1242,13 +1251,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2275,7 +2278,7 @@
       <c r="D20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2462,25 +2465,25 @@
       <c r="C31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="I31" s="16" t="s">
+      <c r="I31" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="14" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2488,13 +2491,13 @@
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="16">
         <v>43873</v>
       </c>
       <c r="C32" s="1">
         <v>120</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="16">
         <f>B32+C32</f>
         <v>43993</v>
       </c>
@@ -2514,7 +2517,7 @@
         <f>TEXT(D32,"DDDD")</f>
         <v>Thursday</v>
       </c>
-      <c r="I32" s="16" t="str">
+      <c r="I32" s="15" t="str">
         <f>TEXT(D32,"MMMM")</f>
         <v>June</v>
       </c>
@@ -2527,13 +2530,13 @@
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <v>44269</v>
       </c>
       <c r="C33" s="1">
         <v>70</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="16">
         <f t="shared" ref="D33:D37" si="4">B33+C33</f>
         <v>44339</v>
       </c>
@@ -2553,7 +2556,7 @@
         <f t="shared" ref="H33:H37" si="8">TEXT(D33,"DDDD")</f>
         <v>Sunday</v>
       </c>
-      <c r="I33" s="16" t="str">
+      <c r="I33" s="15" t="str">
         <f t="shared" ref="I33:I37" si="9">TEXT(D33,"MMMM")</f>
         <v>May</v>
       </c>
@@ -2566,13 +2569,13 @@
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="16">
         <v>44341</v>
       </c>
       <c r="C34" s="1">
         <v>123</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="16">
         <f t="shared" si="4"/>
         <v>44464</v>
       </c>
@@ -2592,7 +2595,7 @@
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="I34" s="16" t="str">
+      <c r="I34" s="15" t="str">
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
@@ -2605,13 +2608,13 @@
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="16">
         <v>44418</v>
       </c>
       <c r="C35" s="1">
         <v>90</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="16">
         <f t="shared" si="4"/>
         <v>44508</v>
       </c>
@@ -2631,7 +2634,7 @@
         <f t="shared" si="8"/>
         <v>Monday</v>
       </c>
-      <c r="I35" s="16" t="str">
+      <c r="I35" s="15" t="str">
         <f t="shared" si="9"/>
         <v>November</v>
       </c>
@@ -2644,13 +2647,13 @@
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="16">
         <v>44571</v>
       </c>
       <c r="C36" s="1">
         <v>89</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="16">
         <f t="shared" si="4"/>
         <v>44660</v>
       </c>
@@ -2670,7 +2673,7 @@
         <f t="shared" si="8"/>
         <v>Saturday</v>
       </c>
-      <c r="I36" s="16" t="str">
+      <c r="I36" s="15" t="str">
         <f t="shared" si="9"/>
         <v>April</v>
       </c>
@@ -2683,13 +2686,13 @@
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>44594</v>
       </c>
       <c r="C37" s="1">
         <v>250</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="16">
         <f t="shared" si="4"/>
         <v>44844</v>
       </c>
@@ -2709,7 +2712,7 @@
         <f t="shared" si="8"/>
         <v>Monday</v>
       </c>
-      <c r="I37" s="16" t="str">
+      <c r="I37" s="15" t="str">
         <f t="shared" si="9"/>
         <v>October</v>
       </c>
@@ -2727,7 +2730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A468B79F-181A-4FE7-BD7B-354CCF492C7F}">
   <dimension ref="C1:J98"/>
   <sheetViews>
-    <sheetView topLeftCell="C84" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
@@ -5275,7 +5278,7 @@
   <dimension ref="A2:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5340,20 +5343,20 @@
         <f>VLOOKUP(F8,'Exercise 3 Q.1(6 July 23 Thur)'!C2:J98,7,)</f>
         <v>31467</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15" t="s">
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="S8" s="15" t="s">
+      <c r="S8" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="T8" s="15" t="s">
+      <c r="T8" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="U8" s="15"/>
+      <c r="U8" s="14"/>
     </row>
     <row r="9" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F9" s="6">
@@ -5535,16 +5538,16 @@
       <c r="J21" s="11">
         <v>5</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="L21" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="25" t="s">
         <v>276</v>
       </c>
-      <c r="N21" s="13" t="s">
+      <c r="N21" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="O21" s="13" t="s">
+      <c r="O21" s="25" t="s">
         <v>278</v>
       </c>
     </row>
@@ -5567,18 +5570,18 @@
       <c r="J22" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="11">
         <v>3</v>
       </c>
-      <c r="M22">
-        <f>HLOOKUP(H21,E21:J24,4,)</f>
+      <c r="M22" s="1">
+        <f>HLOOKUP(L22,$E$21:$J$24,4,)</f>
         <v>90</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="1">
         <f>HLOOKUP(L22,$E$21:$J$24,3,)</f>
         <v>50</v>
       </c>
-      <c r="O22" t="str">
+      <c r="O22" s="1" t="str">
         <f>HLOOKUP(L22,$E$21:$J$24,2,)</f>
         <v>c</v>
       </c>
@@ -5602,18 +5605,18 @@
       <c r="J23" s="11">
         <v>46</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="11">
         <v>1</v>
       </c>
-      <c r="M23">
-        <f>HLOOKUP(F21,E21:J24,4,)</f>
+      <c r="M23" s="1">
+        <f>HLOOKUP(L23,$E$21:$J$24,4,)</f>
         <v>56</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="1">
         <f>HLOOKUP(L23,$E$21:$J$24,3,)</f>
         <v>45</v>
       </c>
-      <c r="O23" t="str">
+      <c r="O23" s="1" t="str">
         <f>HLOOKUP(L23,$E$21:$J$24,2,)</f>
         <v>a</v>
       </c>
@@ -5655,23 +5658,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5922DC4-94E9-454B-BBB5-FED1D6ACACBB}">
-  <dimension ref="H3:U18"/>
+  <dimension ref="H3:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H3" s="8" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="8:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="T4" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H5" s="9" t="s">
         <v>83</v>
       </c>
@@ -5688,13 +5700,22 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="8:21" x14ac:dyDescent="0.3">
-      <c r="H6" s="24" t="s">
+    <row r="6" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="H6" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="I6" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H6,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>41</v>
+      </c>
+      <c r="J6" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H6,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>6'3</v>
+      </c>
+      <c r="K6" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H6,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Men</v>
+      </c>
       <c r="L6" s="6"/>
       <c r="O6" s="11" t="s">
         <v>275</v>
@@ -5715,13 +5736,22 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H7" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="I7" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H7,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>42</v>
+      </c>
+      <c r="J7" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H7,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>6'1</v>
+      </c>
+      <c r="K7" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H7,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Men</v>
+      </c>
       <c r="L7" s="6"/>
       <c r="O7" s="11">
         <v>1</v>
@@ -5738,14 +5768,27 @@
       <c r="T7" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="8:21" x14ac:dyDescent="0.3">
+      <c r="U7" t="str">
+        <f>INDEX($O$6:$R$11,3,2)</f>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="8" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H8" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="I8" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H8,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>43</v>
+      </c>
+      <c r="J8" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H8,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>6'1</v>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H8,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Men</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="O8" s="11">
         <v>2</v>
@@ -5763,13 +5806,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H9" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="I9" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H9,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>22</v>
+      </c>
+      <c r="J9" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H9,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>5'8</v>
+      </c>
+      <c r="K9" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H9,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Women</v>
+      </c>
       <c r="L9" s="6"/>
       <c r="O9" s="11">
         <v>3</v>
@@ -5784,13 +5836,22 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H10" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="I10" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H10,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>23</v>
+      </c>
+      <c r="J10" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H10,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>5'9</v>
+      </c>
+      <c r="K10" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H10,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Women</v>
+      </c>
       <c r="L10" s="6"/>
       <c r="O10" s="11">
         <v>4</v>
@@ -5805,13 +5866,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H11" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="I11" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H11,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>30</v>
+      </c>
+      <c r="J11" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H11,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>6'2</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H11,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Men</v>
+      </c>
       <c r="L11" s="6"/>
       <c r="O11" s="11">
         <v>5</v>
@@ -5826,17 +5896,26 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="8:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H12" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="I12" s="19">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H12,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),1)</f>
+        <v>31</v>
+      </c>
+      <c r="J12" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!C$2:J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H12,'Exercise 3 Q.1(6 July 23 Thur)'!F$2:F$98,0),6)</f>
+        <v>6'2</v>
+      </c>
+      <c r="K12" s="6" t="str">
+        <f>INDEX('Exercise 3 Q.1(6 July 23 Thur)'!$C$2:$J$98,MATCH('Exercise 3 Q.3(4 July 23)'!H12,'Exercise 3 Q.1(6 July 23 Thur)'!$F$2:$F$98,0),2)</f>
+        <v>Men</v>
+      </c>
       <c r="L12" s="6"/>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J18" s="23"/>
+      <c r="J18" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5854,56 +5933,56 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="5:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="6" spans="5:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="19"/>
-      <c r="K6" s="14" t="s">
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="21"/>
+      <c r="K6" s="13" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="8" spans="5:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="19"/>
-      <c r="K8" s="14" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="21"/>
+      <c r="K8" s="13" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="10" spans="5:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="19"/>
-      <c r="K10" s="14" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
+      <c r="K10" s="13" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="12" spans="5:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="19"/>
-      <c r="K12" s="14" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="21"/>
+      <c r="K12" s="13" t="s">
         <v>294</v>
       </c>
     </row>

</xml_diff>